<commit_message>
Final hand in StepperMain file
The final file for the stepper main file
</commit_message>
<xml_diff>
--- a/Stepper Code Tests/Results.xlsx
+++ b/Stepper Code Tests/Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,6 +165,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1939,11 +1939,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-845314976"/>
-        <c:axId val="-845313888"/>
+        <c:axId val="1226179424"/>
+        <c:axId val="1226179968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-845314976"/>
+        <c:axId val="1226179424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2000,12 +2000,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-845313888"/>
+        <c:crossAx val="1226179968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-845313888"/>
+        <c:axId val="1226179968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2062,7 +2062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-845314976"/>
+        <c:crossAx val="1226179424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2076,6 +2076,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2157,6 +2158,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3440,11 +3442,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-845311712"/>
-        <c:axId val="-845309536"/>
+        <c:axId val="1226190304"/>
+        <c:axId val="1226187584"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-845311712"/>
+        <c:axId val="1226190304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3501,12 +3503,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-845309536"/>
+        <c:crossAx val="1226187584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-845309536"/>
+        <c:axId val="1226187584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3563,7 +3565,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-845311712"/>
+        <c:crossAx val="1226190304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3577,6 +3579,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8498,11 +8501,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-845307360"/>
-        <c:axId val="-911237568"/>
+        <c:axId val="1226181600"/>
+        <c:axId val="1226188128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-845307360"/>
+        <c:axId val="1226181600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8559,12 +8562,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-911237568"/>
+        <c:crossAx val="1226188128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-911237568"/>
+        <c:axId val="1226188128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8621,7 +8624,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-845307360"/>
+        <c:crossAx val="1226181600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8717,6 +8720,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9470,11 +9474,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-911239744"/>
-        <c:axId val="-911232672"/>
+        <c:axId val="1226183776"/>
+        <c:axId val="1226189216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-911239744"/>
+        <c:axId val="1226183776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9531,12 +9535,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-911232672"/>
+        <c:crossAx val="1226189216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-911232672"/>
+        <c:axId val="1226189216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9593,7 +9597,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-911239744"/>
+        <c:crossAx val="1226183776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9607,6 +9611,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13487,7 +13492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -14309,7 +14314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J394"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>

</xml_diff>